<commit_message>
eliminando logo del archivo base
</commit_message>
<xml_diff>
--- a/BASEXLSMCODCOLOR.xlsx
+++ b/BASEXLSMCODCOLOR.xlsx
@@ -280,58 +280,28 @@
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -361,6 +331,36 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -377,61 +377,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>281483</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1056862</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>91522</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E089C173-1453-8A9F-ACF8-10567234CC5A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="281483" y="76200"/>
-          <a:ext cx="775379" cy="834472"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -713,149 +658,144 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="19"/>
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="20"/>
+      <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="7" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8" t="s">
+      <c r="H2" s="25"/>
+      <c r="I2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="21"/>
+      <c r="B3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="5" t="s">
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="17"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="19" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="21"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="11"/>
     </row>
     <row r="8" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="25" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="27"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="17"/>
     </row>
-    <row r="9" spans="1:9" ht="42" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+    <row r="9" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:I8"/>
     <mergeCell ref="G9:I9"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:F1"/>
@@ -864,8 +804,12 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="G3:I3"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>